<commit_message>
CHECKER DONE week13 end
</commit_message>
<xml_diff>
--- a/Review.xlsx
+++ b/Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>Дата</t>
   </si>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,9 +422,11 @@
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +466,14 @@
       <c r="M1" s="4">
         <v>42331</v>
       </c>
+      <c r="N1" s="4">
+        <v>42338</v>
+      </c>
+      <c r="O1" s="4">
+        <v>42345</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -499,8 +507,14 @@
       <c r="M2" t="s">
         <v>6</v>
       </c>
+      <c r="N2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -533,6 +547,12 @@
       </c>
       <c r="M3" t="s">
         <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
template for last week
</commit_message>
<xml_diff>
--- a/Review.xlsx
+++ b/Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>Дата</t>
   </si>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,9 +424,11 @@
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,8 +474,14 @@
       <c r="O1" s="4">
         <v>42345</v>
       </c>
+      <c r="P1" s="4">
+        <v>42352</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>42359</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -513,8 +521,14 @@
       <c r="O2" t="s">
         <v>10</v>
       </c>
+      <c r="P2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -553,6 +567,12 @@
       </c>
       <c r="O3" t="s">
         <v>6</v>
+      </c>
+      <c r="P3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>